<commit_message>
annotating correspondence between xlinks and RESID; removing residues that represent xlinks from alphabet
</commit_message>
<xml_diff>
--- a/bpforms/xlink/xlink.xlsx
+++ b/bpforms/xlink/xlink.xlsx
@@ -1,37 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoyuezheng/Desktop/karrlab/projects/bcforms/bcforms/xlink/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951D16B8-861F-5E45-B3BA-81944D79E7ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="920" windowWidth="27640" windowHeight="16200" xr2:uid="{091FBCF7-AB49-3546-8B60-F04EB334A316}"/>
+    <workbookView windowWidth="28695" windowHeight="13965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="284">
   <si>
     <t>index</t>
   </si>
@@ -63,6 +46,9 @@
     <t>xlink_SMILES</t>
   </si>
   <si>
+    <t>left_monomer_alphabet</t>
+  </si>
+  <si>
     <t>left_monomer</t>
   </si>
   <si>
@@ -75,6 +61,9 @@
     <t>left_SMILES</t>
   </si>
   <si>
+    <t>right_monomer_alphabet</t>
+  </si>
+  <si>
     <t>right_monomer</t>
   </si>
   <si>
@@ -87,12 +76,27 @@
     <t>right_SMILES</t>
   </si>
   <si>
+    <t>alphabet</t>
+  </si>
+  <si>
+    <t>alphabet_id</t>
+  </si>
+  <si>
+    <t>resid_id</t>
+  </si>
+  <si>
+    <t>A,C</t>
+  </si>
+  <si>
     <t>2-(L-cystein-S-yl)-L-alanine</t>
   </si>
   <si>
     <t>O=C[C@H](CS[C@](C(=O)O)(N)C)[NH3+]</t>
   </si>
   <si>
+    <t>bpforms.ProteinForm</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -117,9 +121,21 @@
     <t>OC(=O)[C@@H]([NH3+])CS</t>
   </si>
   <si>
+    <t>protein</t>
+  </si>
+  <si>
+    <t>A, C</t>
+  </si>
+  <si>
+    <t>AA0621</t>
+  </si>
+  <si>
     <t>AA0025</t>
   </si>
   <si>
+    <t>C,C</t>
+  </si>
+  <si>
     <t>L-cystine</t>
   </si>
   <si>
@@ -132,9 +148,15 @@
     <t>AA0126</t>
   </si>
   <si>
+    <t>D,G</t>
+  </si>
+  <si>
     <t>N-(L-isoaspartyl)-glycine</t>
   </si>
   <si>
+    <t>isoaspartyl_glycine_isopeptide</t>
+  </si>
+  <si>
     <t>isopeptide</t>
   </si>
   <si>
@@ -168,9 +190,15 @@
     <t>AA0206</t>
   </si>
   <si>
+    <t>G,C</t>
+  </si>
+  <si>
     <t>S-glycyl-L-cysteine</t>
   </si>
   <si>
+    <t>glycine_cysteine_thioester</t>
+  </si>
+  <si>
     <t>thioester</t>
   </si>
   <si>
@@ -183,9 +211,15 @@
     <t>AA0360</t>
   </si>
   <si>
+    <t>G,E</t>
+  </si>
+  <si>
     <t>N-(L-isoglutamyl)-glycine</t>
   </si>
   <si>
+    <t>isoglutamyl_glycine_isopeptide</t>
+  </si>
+  <si>
     <t>O=C[C@H](CCC(=O)NCC(=O)O)[NH3+]</t>
   </si>
   <si>
@@ -204,6 +238,9 @@
     <t>AA0368</t>
   </si>
   <si>
+    <t>Y,Y</t>
+  </si>
+  <si>
     <t>3'-(L-tyros-O4'-yl)-L-tyrosine</t>
   </si>
   <si>
@@ -234,6 +271,9 @@
     <t>S-(L-alanyl)-L-cysteine</t>
   </si>
   <si>
+    <t>alanine_cysteine_thioester</t>
+  </si>
+  <si>
     <t>C[C@H]([NH3+])C(=O)SC[C@@H](C(=O)O)N</t>
   </si>
   <si>
@@ -246,9 +286,15 @@
     <t>AA0413</t>
   </si>
   <si>
+    <t>C,M</t>
+  </si>
+  <si>
     <t>S-(L-methionyl)-L-cysteine</t>
   </si>
   <si>
+    <t>methionine_cysteine_thioester</t>
+  </si>
+  <si>
     <t>CSCC[C@@H](C(=O)SC[C@@H](C(=O)O)N)[NH3+]</t>
   </si>
   <si>
@@ -267,9 +313,15 @@
     <t>AA0414</t>
   </si>
   <si>
+    <t>F,C</t>
+  </si>
+  <si>
     <t>S-(L-phenylalanyl)-L-cysteine</t>
   </si>
   <si>
+    <t>phenylalanine_cysteine_thioester</t>
+  </si>
+  <si>
     <t>[NH3+][C@H](C(=O)SC[C@@H](C(=O)O)N)Cc1ccccc1</t>
   </si>
   <si>
@@ -285,9 +337,15 @@
     <t>AA0415</t>
   </si>
   <si>
+    <t>T,C</t>
+  </si>
+  <si>
     <t>S-(L-threonyl)-L-cysteine</t>
   </si>
   <si>
+    <t>threonine_cysteine_thioester</t>
+  </si>
+  <si>
     <t>C[C@H]([C@@H](C(=O)SC[C@@H](C(=O)O)N)[NH3+])O</t>
   </si>
   <si>
@@ -303,18 +361,30 @@
     <t>AA0416</t>
   </si>
   <si>
+    <t>Y,C</t>
+  </si>
+  <si>
     <t>S-(L-tyrosyl)-L-cysteine</t>
   </si>
   <si>
+    <t>tyrosine_cysteine_thioester</t>
+  </si>
+  <si>
     <t>O=C([C@H](Cc1ccc(cc1)O)[NH3+])SC[C@@H](C(=O)O)N</t>
   </si>
   <si>
     <t>AA0417</t>
   </si>
   <si>
+    <t>W,C</t>
+  </si>
+  <si>
     <t>S-(L-tryptophanyl)-L-cysteine</t>
   </si>
   <si>
+    <t>tryptophan_cysteine_thioester</t>
+  </si>
+  <si>
     <t>O=C([C@H](Cc1c[nH]c2c1cccc2)[NH3+])SC[C@@H](C(=O)O)N</t>
   </si>
   <si>
@@ -327,9 +397,15 @@
     <t>AA0495</t>
   </si>
   <si>
+    <t>G,S</t>
+  </si>
+  <si>
     <t>O-glycyl-L-serine</t>
   </si>
   <si>
+    <t>serine_glycinate_ester</t>
+  </si>
+  <si>
     <t>ester</t>
   </si>
   <si>
@@ -351,6 +427,9 @@
     <t>AA0505</t>
   </si>
   <si>
+    <t>E,K</t>
+  </si>
+  <si>
     <t>N2-(L-isoglutamyl)-L-lysine</t>
   </si>
   <si>
@@ -372,6 +451,9 @@
     <t>AA0536</t>
   </si>
   <si>
+    <t>T,Q</t>
+  </si>
+  <si>
     <t>O-(isoglutamyl)-L-threonine</t>
   </si>
   <si>
@@ -390,6 +472,9 @@
     <t>AA0586</t>
   </si>
   <si>
+    <t>K,K</t>
+  </si>
+  <si>
     <t>L-lysinonorleucine</t>
   </si>
   <si>
@@ -405,6 +490,9 @@
     <t>N1-1, H1+1, H1, H1</t>
   </si>
   <si>
+    <t>C,D</t>
+  </si>
+  <si>
     <t>3-(S-L-cysteinyl)-L-aspartic acid</t>
   </si>
   <si>
@@ -414,9 +502,21 @@
     <t>H5</t>
   </si>
   <si>
+    <t>C, D</t>
+  </si>
+  <si>
+    <t>AA0314</t>
+  </si>
+  <si>
+    <t>C,L</t>
+  </si>
+  <si>
     <t>S-(L-leucyl)-L-cysteine</t>
   </si>
   <si>
+    <t>leucine_cysteine_thioester</t>
+  </si>
+  <si>
     <t>[NH3+][C@H](C(=O)SC[C@@H](C(=O)O)N)CC(C)C</t>
   </si>
   <si>
@@ -426,18 +526,45 @@
     <t>[NH3+][C@H](C(=O)O)CC(C)C</t>
   </si>
   <si>
+    <t>C, L</t>
+  </si>
+  <si>
+    <t>AA0412</t>
+  </si>
+  <si>
     <t>2-(L-cystein-S-yl)-L-methionine</t>
   </si>
   <si>
     <t>CSCC[C@@](SC[C@@H](C(=O)O)[NH3+])(C=O)N</t>
   </si>
   <si>
+    <t>C, M</t>
+  </si>
+  <si>
+    <t>AA0559</t>
+  </si>
+  <si>
+    <t>C,Q</t>
+  </si>
+  <si>
     <t>S-(L-isoglutamyl)-L-cysteine</t>
   </si>
   <si>
+    <t>isoglutamyl_cysteine_thioester</t>
+  </si>
+  <si>
     <t>O=C[C@H](CCC(=O)SC[C@@H](C(=O)O)N)[NH3+]</t>
   </si>
   <si>
+    <t>C, Q</t>
+  </si>
+  <si>
+    <t>AA0108</t>
+  </si>
+  <si>
+    <t>C,S</t>
+  </si>
+  <si>
     <t>2-(L-cystein-S-yl)-L-serine</t>
   </si>
   <si>
@@ -450,6 +577,15 @@
     <t>H3</t>
   </si>
   <si>
+    <t>C, S</t>
+  </si>
+  <si>
+    <t>AA0623</t>
+  </si>
+  <si>
+    <t>C,Y</t>
+  </si>
+  <si>
     <t>2-(L-cystein-S-yl)-D-tyrosine</t>
   </si>
   <si>
@@ -462,6 +598,15 @@
     <t>H4</t>
   </si>
   <si>
+    <t>C, Y</t>
+  </si>
+  <si>
+    <t>AA0626</t>
+  </si>
+  <si>
+    <t>D,K</t>
+  </si>
+  <si>
     <t>N6-(L-aspartyl)-L-lysine</t>
   </si>
   <si>
@@ -474,24 +619,69 @@
     <t>H1+1, H1</t>
   </si>
   <si>
+    <t>D, K</t>
+  </si>
+  <si>
+    <t>AA0583</t>
+  </si>
+  <si>
+    <t>D,T</t>
+  </si>
+  <si>
     <t>O-isoaspartyl-L-threonine</t>
   </si>
   <si>
+    <t>threonine_aspartic_ester</t>
+  </si>
+  <si>
     <t>O=C[C@H]([C@H](OC(=O)C[C@@H](C(=O)[O-])[NH3+])C)[NH3+]</t>
   </si>
   <si>
+    <t>D, T</t>
+  </si>
+  <si>
+    <t>AA0525</t>
+  </si>
+  <si>
+    <t>E,S</t>
+  </si>
+  <si>
     <t>O-(L-isoglutamyl)-L-serine</t>
   </si>
   <si>
+    <t>isoglutamyl_serine_ester</t>
+  </si>
+  <si>
     <t>O=C[C@H](CCC(=O)OC[C@@H](C(=O)O)N)[NH3+]</t>
   </si>
   <si>
+    <t>E, S</t>
+  </si>
+  <si>
+    <t>AA0597</t>
+  </si>
+  <si>
+    <t>F,S</t>
+  </si>
+  <si>
     <t>O-(L-phenylalanyl)-L-serine</t>
   </si>
   <si>
+    <t>phenylalanine_serine_ester</t>
+  </si>
+  <si>
     <t>N[C@H](C(=O)OC[C@@H](C(=O)O)[NH3+])Cc1ccccc1</t>
   </si>
   <si>
+    <t>F, S</t>
+  </si>
+  <si>
+    <t>AA0418</t>
+  </si>
+  <si>
+    <t>F,V</t>
+  </si>
+  <si>
     <t>3-(L-phenylalan-2'-yl)-L-valine</t>
   </si>
   <si>
@@ -510,21 +700,57 @@
     <t>[NH3+]C(C(=O)O)C(C)C</t>
   </si>
   <si>
+    <t>F, V</t>
+  </si>
+  <si>
+    <t>AA0565</t>
+  </si>
+  <si>
+    <t>G,K</t>
+  </si>
+  <si>
     <t>N6-glycyl-L-lysine</t>
   </si>
   <si>
+    <t>glycyl_lysine_isopeptide</t>
+  </si>
+  <si>
     <t>[NH3+]CC(=O)NCCCC[C@@H](C(=O)O)[NH3+]</t>
   </si>
   <si>
+    <t>G, K</t>
+  </si>
+  <si>
+    <t>AA0125</t>
+  </si>
+  <si>
+    <t>G,T</t>
+  </si>
+  <si>
     <t>O-glycyl-L-threonine</t>
   </si>
   <si>
+    <t>threonine_glycinate_ester</t>
+  </si>
+  <si>
     <t>C[C@H]([C@H]([NH3+])C(=O)O)OC(=O)CN</t>
   </si>
   <si>
+    <t>G, T</t>
+  </si>
+  <si>
+    <t>AA0496</t>
+  </si>
+  <si>
+    <t>K,N</t>
+  </si>
+  <si>
     <t>N6-(L-isoaspartyl)-L-lysine</t>
   </si>
   <si>
+    <t>isoaspartyl_lysine_isopeptide</t>
+  </si>
+  <si>
     <t>O=C[C@H](CCCCNC(=O)C[C@@H](C(=O)O)N)[NH3+]</t>
   </si>
   <si>
@@ -534,24 +760,63 @@
     <t>NC(=O)C[C@@H](C(=O)O)[NH3+]</t>
   </si>
   <si>
+    <t>K, N</t>
+  </si>
+  <si>
+    <t>AA0294</t>
+  </si>
+  <si>
+    <t>K,Q</t>
+  </si>
+  <si>
     <t>N6-(L-isoglutamyl)-L-lysine</t>
   </si>
   <si>
+    <t>isoglutamyl_lysine_isopeptide</t>
+  </si>
+  <si>
     <t>O=C[C@H](CCCCNC(=O)CC[C@@H](C(=O)O)[NH3+])[NH3+]</t>
   </si>
   <si>
+    <t>K, Q</t>
+  </si>
+  <si>
+    <t>AA0124</t>
+  </si>
+  <si>
+    <t>K,S</t>
+  </si>
+  <si>
     <t>L-lysinoalanine</t>
   </si>
   <si>
     <t>O=C[C@H](CCCC[NH2+]C[C@@H](C(=O)O)N)[NH3+]</t>
   </si>
   <si>
+    <t>K, S</t>
+  </si>
+  <si>
+    <t>AA0123</t>
+  </si>
+  <si>
+    <t>K,T</t>
+  </si>
+  <si>
     <t>N6-(L-threonyl)-L-lysine</t>
   </si>
   <si>
     <t>[NH3+][C@H](C(=O)NCCCC[C@@H](C(=O)O)[NH3+])[C@H](O)C</t>
   </si>
   <si>
+    <t>K, T</t>
+  </si>
+  <si>
+    <t>AA0440</t>
+  </si>
+  <si>
+    <t>U,U</t>
+  </si>
+  <si>
     <t>L-selenocystine</t>
   </si>
   <si>
@@ -570,205 +835,418 @@
     <t>N[C@H](C(=O)O)C[SeH]</t>
   </si>
   <si>
+    <t>U, U</t>
+  </si>
+  <si>
+    <t>AA0437</t>
+  </si>
+  <si>
+    <t>V,Y</t>
+  </si>
+  <si>
     <t>3-(O4'-L-tyrosyl)-L-valine</t>
   </si>
   <si>
     <t>O=C[C@H](Cc1ccc(cc1)OC([C@@H](C(=O)O)[NH3+])(C)C)[NH3+]</t>
   </si>
   <si>
+    <t>V, Y</t>
+  </si>
+  <si>
+    <t>AA0490</t>
+  </si>
+  <si>
     <t>3'-(L-tyros-3'-yl)-L-tyrosine</t>
   </si>
   <si>
     <t>O=C[C@H](Cc1ccc(c(c1)c1cc(ccc1O)C[C@@H](C(=O)O)[NH3+])O)[NH3+]</t>
   </si>
   <si>
-    <t>A,C</t>
-  </si>
-  <si>
-    <t>C,D</t>
-  </si>
-  <si>
-    <t>C,L</t>
-  </si>
-  <si>
-    <t>C,M</t>
-  </si>
-  <si>
-    <t>C,Q</t>
-  </si>
-  <si>
-    <t>C,S</t>
-  </si>
-  <si>
-    <t>C,Y</t>
-  </si>
-  <si>
-    <t>D,K</t>
-  </si>
-  <si>
-    <t>D,T</t>
-  </si>
-  <si>
-    <t>E,S</t>
-  </si>
-  <si>
-    <t>F,S</t>
-  </si>
-  <si>
-    <t>F,V</t>
-  </si>
-  <si>
-    <t>G,K</t>
-  </si>
-  <si>
-    <t>G,T</t>
-  </si>
-  <si>
-    <t>K,N</t>
-  </si>
-  <si>
-    <t>K,Q</t>
-  </si>
-  <si>
-    <t>K,S</t>
-  </si>
-  <si>
-    <t>K,T</t>
-  </si>
-  <si>
-    <t>U,U</t>
-  </si>
-  <si>
-    <t>V,Y</t>
-  </si>
-  <si>
-    <t>Y,Y</t>
-  </si>
-  <si>
-    <t>C,C</t>
-  </si>
-  <si>
-    <t>D,G</t>
-  </si>
-  <si>
-    <t>G,C</t>
-  </si>
-  <si>
-    <t>G,E</t>
-  </si>
-  <si>
-    <t>F,C</t>
-  </si>
-  <si>
-    <t>T,C</t>
-  </si>
-  <si>
-    <t>Y,C</t>
-  </si>
-  <si>
-    <t>W,C</t>
-  </si>
-  <si>
-    <t>G,S</t>
-  </si>
-  <si>
-    <t>E,K</t>
-  </si>
-  <si>
-    <t>T,Q</t>
-  </si>
-  <si>
-    <t>K,K</t>
-  </si>
-  <si>
-    <t>glycine_cysteine_thioester</t>
-  </si>
-  <si>
-    <t>isoglutamyl_glycine_isopeptide</t>
-  </si>
-  <si>
-    <t>alanine_cysteine_thioester</t>
-  </si>
-  <si>
-    <t>methionine_cysteine_thioester</t>
-  </si>
-  <si>
-    <t>phenylalanine_cysteine_thioester</t>
-  </si>
-  <si>
-    <t>threonine_cysteine_thioester</t>
-  </si>
-  <si>
-    <t>tyrosine_cysteine_thioester</t>
-  </si>
-  <si>
-    <t>tryptophan_cysteine_thioester</t>
-  </si>
-  <si>
-    <t>serine_glycinate_ester</t>
-  </si>
-  <si>
-    <t>leucine_cysteine_thioester</t>
-  </si>
-  <si>
-    <t>isoglutamyl_cysteine_thioester</t>
-  </si>
-  <si>
-    <t>threonine_aspartic_ester</t>
-  </si>
-  <si>
-    <t>isoglutamyl_serine_ester</t>
-  </si>
-  <si>
-    <t>phenylalanine_serine_ester</t>
-  </si>
-  <si>
-    <t>threonine_glycinate_ester</t>
-  </si>
-  <si>
-    <t>isoaspartyl_lysine_isopeptide</t>
-  </si>
-  <si>
-    <t>isoglutamyl_lysine_isopeptide</t>
-  </si>
-  <si>
-    <t>isoaspartyl_glycine_isopeptide</t>
-  </si>
-  <si>
-    <t>glycyl_lysine_isopeptide</t>
-  </si>
-  <si>
-    <t>left_monomer_alphabet</t>
-  </si>
-  <si>
-    <t>bpforms.ProteinForm</t>
-  </si>
-  <si>
-    <t>right_monomer_alphabet</t>
+    <t>Y, Y</t>
+  </si>
+  <si>
+    <t>AA0367</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -776,27 +1254,315 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -807,10 +1573,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="212121"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="F3F3F3"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -845,7 +1611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -878,26 +1644,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -930,23 +1679,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1088,1150 +1820,1347 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D26CF6B-E6EE-114C-9D76-237F535B67EE}">
-  <dimension ref="A1:T37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>235</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T2" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" t="s">
-        <v>236</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="P3" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T3" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>233</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R4" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4" t="s">
+        <v>55</v>
+      </c>
+      <c r="T4" t="s">
+        <v>56</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K4" t="s">
-        <v>236</v>
-      </c>
-      <c r="L4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" t="s">
-        <v>41</v>
-      </c>
-      <c r="S4" t="s">
-        <v>42</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>43</v>
       </c>
+      <c r="W4" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>216</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="K5" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="M5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="O5" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="P5" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T5" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>207</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="K6" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="M6" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="N6" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="O6" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="P6" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q6" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="R6" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="S6" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="T6" t="s">
-        <v>55</v>
+        <v>72</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W6" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="A7">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>203</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="M7" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="N7" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="O7" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="P7" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q7" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="R7" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="S7" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="T7" t="s">
-        <v>62</v>
+        <v>80</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V7" t="s">
+        <v>73</v>
+      </c>
+      <c r="W7" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="A8">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>218</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="K8" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="N8" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="O8" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="P8" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q8" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R8" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T8" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V8" t="s">
+        <v>83</v>
+      </c>
+      <c r="W8" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="A9">
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
-        <v>219</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J9" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="K9" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="M9" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="P9" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q9" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="R9" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="S9" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="T9" t="s">
-        <v>76</v>
+        <v>97</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V9" t="s">
+        <v>89</v>
+      </c>
+      <c r="W9" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23">
       <c r="A10">
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>208</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>220</v>
+        <v>101</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J10" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="K10" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L10" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="M10" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="N10" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="O10" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="P10" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T10" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V10" t="s">
+        <v>98</v>
+      </c>
+      <c r="W10" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23">
       <c r="A11">
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>221</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J11" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="K11" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L11" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="M11" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="N11" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="O11" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="P11" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q11" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R11" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T11" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V11" t="s">
+        <v>106</v>
+      </c>
+      <c r="W11" t="s">
+        <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23">
       <c r="A12">
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
-        <v>210</v>
+        <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="E12" t="s">
-        <v>222</v>
+        <v>117</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J12" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="K12" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="M12" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="N12" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="O12" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="P12" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R12" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S12" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T12" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V12" t="s">
+        <v>114</v>
+      </c>
+      <c r="W12" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23">
       <c r="A13">
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="E13" t="s">
-        <v>223</v>
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J13" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="K13" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L13" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="M13" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="N13" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="O13" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="P13" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q13" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R13" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T13" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V13" t="s">
+        <v>119</v>
+      </c>
+      <c r="W13" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23">
       <c r="A14">
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
-        <v>212</v>
+        <v>127</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="E14" t="s">
-        <v>224</v>
+        <v>129</v>
       </c>
       <c r="F14" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="J14" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="K14" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L14" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="M14" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="N14" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="O14" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="P14" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q14" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="R14" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="S14" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="T14" t="s">
-        <v>104</v>
+        <v>135</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V14" t="s">
+        <v>126</v>
+      </c>
+      <c r="W14" t="s">
+        <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23">
       <c r="A15">
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>137</v>
       </c>
       <c r="D15" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="J15" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="K15" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L15" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="M15" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="N15" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="O15" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="P15" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q15" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="R15" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="S15" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="T15" t="s">
-        <v>111</v>
+        <v>143</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V15" t="s">
+        <v>136</v>
+      </c>
+      <c r="W15" t="s">
+        <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23">
       <c r="A16">
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>214</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
+        <v>146</v>
+      </c>
+      <c r="J16" t="s">
+        <v>147</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" t="s">
+        <v>111</v>
+      </c>
+      <c r="M16" t="s">
+        <v>81</v>
+      </c>
+      <c r="N16" t="s">
+        <v>82</v>
+      </c>
+      <c r="O16" t="s">
         <v>113</v>
       </c>
-      <c r="J16" t="s">
-        <v>114</v>
-      </c>
-      <c r="K16" t="s">
-        <v>236</v>
-      </c>
-      <c r="L16" t="s">
-        <v>86</v>
-      </c>
-      <c r="M16" t="s">
-        <v>63</v>
-      </c>
-      <c r="N16" t="s">
-        <v>64</v>
-      </c>
-      <c r="O16" t="s">
-        <v>88</v>
-      </c>
       <c r="P16" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q16" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="R16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="S16" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="T16" t="s">
-        <v>117</v>
+        <v>150</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V16" t="s">
+        <v>144</v>
+      </c>
+      <c r="W16" t="s">
+        <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23">
       <c r="A17">
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>215</v>
+        <v>152</v>
       </c>
       <c r="D17" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="J17" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="K17" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L17" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="M17" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="N17" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="O17" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="P17" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q17" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="R17" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="S17" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="T17" t="s">
-        <v>111</v>
+        <v>143</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V17" t="s">
+        <v>151</v>
+      </c>
+      <c r="W17" t="s">
+        <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23">
       <c r="A18">
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="J18" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="K18" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L18" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="M18" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N18" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O18" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="P18" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q18" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="R18" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="S18" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="T18" t="s">
-        <v>39</v>
+        <v>52</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V18" t="s">
+        <v>162</v>
+      </c>
+      <c r="W18" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23">
       <c r="A19">
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="C19" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="E19" t="s">
-        <v>225</v>
+        <v>166</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J19" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="K19" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L19" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="M19" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N19" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O19" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="P19" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q19" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="R19" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="S19" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="T19" t="s">
-        <v>130</v>
+        <v>169</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V19" t="s">
+        <v>170</v>
+      </c>
+      <c r="W19" t="s">
+        <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23">
       <c r="A20">
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>186</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>186</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="J20" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="K20" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L20" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="M20" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N20" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O20" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="P20" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q20" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="R20" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="S20" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="T20" t="s">
-        <v>76</v>
+        <v>97</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V20" t="s">
+        <v>174</v>
+      </c>
+      <c r="W20" t="s">
+        <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23">
       <c r="A21">
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C21" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="E21" t="s">
-        <v>226</v>
+        <v>178</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="K21" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L21" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="M21" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N21" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O21" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="P21" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q21" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="R21" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="S21" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="T21" t="s">
-        <v>117</v>
+        <v>150</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V21" t="s">
+        <v>180</v>
+      </c>
+      <c r="W21" t="s">
+        <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23">
       <c r="A22">
         <v>50</v>
       </c>
       <c r="B22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J22" t="s">
+        <v>184</v>
+      </c>
+      <c r="K22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" t="s">
+        <v>33</v>
+      </c>
+      <c r="O22" t="s">
+        <v>34</v>
+      </c>
+      <c r="P22" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>132</v>
+      </c>
+      <c r="R22" t="s">
+        <v>185</v>
+      </c>
+      <c r="S22" t="s">
+        <v>186</v>
+      </c>
+      <c r="T22" t="s">
+        <v>135</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V22" t="s">
+        <v>187</v>
+      </c>
+      <c r="W22" t="s">
         <v>188</v>
       </c>
-      <c r="C22" t="s">
-        <v>188</v>
-      </c>
-      <c r="D22" t="s">
-        <v>135</v>
-      </c>
-      <c r="J22" t="s">
-        <v>136</v>
-      </c>
-      <c r="K22" t="s">
-        <v>236</v>
-      </c>
-      <c r="L22" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N22" t="s">
-        <v>26</v>
-      </c>
-      <c r="O22" t="s">
-        <v>27</v>
-      </c>
-      <c r="P22" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>101</v>
-      </c>
-      <c r="R22" t="s">
-        <v>137</v>
-      </c>
-      <c r="S22" t="s">
-        <v>138</v>
-      </c>
-      <c r="T22" t="s">
-        <v>104</v>
-      </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23">
       <c r="A23">
         <v>55</v>
       </c>
@@ -2242,740 +3171,876 @@
         <v>189</v>
       </c>
       <c r="D23" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="J23" t="s">
-        <v>140</v>
+        <v>191</v>
       </c>
       <c r="K23" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L23" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="M23" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N23" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O23" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="P23" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q23" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="R23" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="S23" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="T23" t="s">
-        <v>62</v>
+        <v>80</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V23" t="s">
+        <v>194</v>
+      </c>
+      <c r="W23" t="s">
+        <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23">
       <c r="A24">
         <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D24" t="s">
+        <v>197</v>
+      </c>
+      <c r="J24" t="s">
+        <v>198</v>
+      </c>
+      <c r="K24" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" t="s">
+        <v>49</v>
+      </c>
+      <c r="M24" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" t="s">
+        <v>52</v>
+      </c>
+      <c r="P24" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>140</v>
+      </c>
+      <c r="R24" t="s">
+        <v>199</v>
+      </c>
+      <c r="S24" t="s">
+        <v>200</v>
+      </c>
+      <c r="T24" t="s">
         <v>143</v>
       </c>
-      <c r="J24" t="s">
-        <v>144</v>
-      </c>
-      <c r="K24" t="s">
-        <v>236</v>
-      </c>
-      <c r="L24" t="s">
-        <v>36</v>
-      </c>
-      <c r="M24" t="s">
-        <v>21</v>
-      </c>
-      <c r="N24" t="s">
-        <v>22</v>
-      </c>
-      <c r="O24" t="s">
-        <v>39</v>
-      </c>
-      <c r="P24" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>108</v>
-      </c>
-      <c r="R24" t="s">
-        <v>145</v>
-      </c>
-      <c r="S24" t="s">
-        <v>146</v>
-      </c>
-      <c r="T24" t="s">
-        <v>111</v>
+      <c r="U24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V24" t="s">
+        <v>201</v>
+      </c>
+      <c r="W24" t="s">
+        <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23">
       <c r="A25">
         <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C25" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="D25" t="s">
-        <v>147</v>
+        <v>204</v>
       </c>
       <c r="E25" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="F25" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="J25" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="K25" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L25" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="M25" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="N25" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="O25" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="P25" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q25" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="R25" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="S25" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="T25" t="s">
-        <v>88</v>
+        <v>113</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V25" t="s">
+        <v>207</v>
+      </c>
+      <c r="W25" t="s">
+        <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23">
       <c r="A26">
         <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="C26" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>210</v>
       </c>
       <c r="E26" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="F26" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="J26" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="K26" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L26" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="M26" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="N26" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="O26" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="P26" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q26" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="R26" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="S26" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="T26" t="s">
-        <v>104</v>
+        <v>135</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V26" t="s">
+        <v>213</v>
+      </c>
+      <c r="W26" t="s">
+        <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23">
       <c r="A27">
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="C27" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>216</v>
       </c>
       <c r="E27" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F27" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="J27" t="s">
-        <v>152</v>
+        <v>218</v>
       </c>
       <c r="K27" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L27" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="M27" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="N27" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="O27" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="P27" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q27" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="R27" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="S27" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="T27" t="s">
-        <v>104</v>
+        <v>135</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V27" t="s">
+        <v>219</v>
+      </c>
+      <c r="W27" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23">
       <c r="A28">
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="C28" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>222</v>
       </c>
       <c r="J28" t="s">
-        <v>154</v>
+        <v>223</v>
       </c>
       <c r="K28" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L28" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="M28" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="N28" t="s">
-        <v>156</v>
+        <v>225</v>
       </c>
       <c r="O28" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="P28" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q28" t="s">
-        <v>157</v>
+        <v>226</v>
       </c>
       <c r="R28" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="S28" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T28" t="s">
-        <v>158</v>
+        <v>227</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V28" t="s">
+        <v>228</v>
+      </c>
+      <c r="W28" t="s">
+        <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23">
       <c r="A29">
         <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="C29" t="s">
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="D29" t="s">
-        <v>159</v>
+        <v>231</v>
       </c>
       <c r="E29" t="s">
+        <v>232</v>
+      </c>
+      <c r="J29" t="s">
+        <v>233</v>
+      </c>
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" t="s">
+        <v>53</v>
+      </c>
+      <c r="M29" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" t="s">
+        <v>63</v>
+      </c>
+      <c r="O29" t="s">
+        <v>56</v>
+      </c>
+      <c r="P29" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>140</v>
+      </c>
+      <c r="R29" t="s">
+        <v>199</v>
+      </c>
+      <c r="S29" t="s">
+        <v>200</v>
+      </c>
+      <c r="T29" t="s">
+        <v>143</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V29" t="s">
         <v>234</v>
       </c>
-      <c r="J29" t="s">
-        <v>160</v>
-      </c>
-      <c r="K29" t="s">
-        <v>236</v>
-      </c>
-      <c r="L29" t="s">
-        <v>40</v>
-      </c>
-      <c r="M29" t="s">
-        <v>21</v>
-      </c>
-      <c r="N29" t="s">
-        <v>48</v>
-      </c>
-      <c r="O29" t="s">
-        <v>43</v>
-      </c>
-      <c r="P29" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>108</v>
-      </c>
-      <c r="R29" t="s">
-        <v>145</v>
-      </c>
-      <c r="S29" t="s">
-        <v>146</v>
-      </c>
-      <c r="T29" t="s">
-        <v>111</v>
+      <c r="W29" t="s">
+        <v>235</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23">
       <c r="A30">
         <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>196</v>
+        <v>236</v>
       </c>
       <c r="C30" t="s">
-        <v>196</v>
+        <v>236</v>
       </c>
       <c r="D30" t="s">
-        <v>161</v>
+        <v>237</v>
       </c>
       <c r="E30" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="F30" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="J30" t="s">
-        <v>162</v>
+        <v>239</v>
       </c>
       <c r="K30" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L30" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="M30" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="N30" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="O30" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="P30" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q30" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="R30" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="S30" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="T30" t="s">
-        <v>88</v>
+        <v>113</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V30" t="s">
+        <v>240</v>
+      </c>
+      <c r="W30" t="s">
+        <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23">
       <c r="A31">
         <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="C31" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="D31" t="s">
-        <v>163</v>
+        <v>243</v>
       </c>
       <c r="E31" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="F31" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="J31" t="s">
-        <v>164</v>
+        <v>245</v>
       </c>
       <c r="K31" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L31" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="M31" t="s">
-        <v>145</v>
+        <v>199</v>
       </c>
       <c r="N31" t="s">
-        <v>146</v>
+        <v>200</v>
       </c>
       <c r="O31" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="P31" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q31" t="s">
-        <v>165</v>
+        <v>246</v>
       </c>
       <c r="R31" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="S31" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="T31" t="s">
-        <v>166</v>
+        <v>247</v>
+      </c>
+      <c r="U31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V31" t="s">
+        <v>248</v>
+      </c>
+      <c r="W31" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23">
       <c r="A32">
         <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>198</v>
+        <v>250</v>
       </c>
       <c r="C32" t="s">
-        <v>198</v>
+        <v>250</v>
       </c>
       <c r="D32" t="s">
-        <v>167</v>
+        <v>251</v>
       </c>
       <c r="E32" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="J32" t="s">
-        <v>168</v>
+        <v>253</v>
       </c>
       <c r="K32" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L32" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="M32" t="s">
-        <v>145</v>
+        <v>199</v>
       </c>
       <c r="N32" t="s">
-        <v>146</v>
+        <v>200</v>
       </c>
       <c r="O32" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="P32" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q32" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="R32" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="S32" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="T32" t="s">
-        <v>117</v>
+        <v>150</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V32" t="s">
+        <v>254</v>
+      </c>
+      <c r="W32" t="s">
+        <v>255</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33">
         <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="C33" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="D33" t="s">
-        <v>169</v>
+        <v>257</v>
       </c>
       <c r="J33" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
       <c r="K33" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L33" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="M33" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="N33" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="O33" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="P33" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q33" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="R33" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="S33" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="T33" t="s">
-        <v>104</v>
+        <v>135</v>
+      </c>
+      <c r="U33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V33" t="s">
+        <v>259</v>
+      </c>
+      <c r="W33" t="s">
+        <v>260</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34">
         <v>82</v>
       </c>
       <c r="B34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D34" t="s">
+        <v>262</v>
+      </c>
+      <c r="J34" t="s">
+        <v>263</v>
+      </c>
+      <c r="K34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" t="s">
+        <v>140</v>
+      </c>
+      <c r="M34" t="s">
+        <v>199</v>
+      </c>
+      <c r="N34" t="s">
         <v>200</v>
       </c>
-      <c r="C34" t="s">
-        <v>200</v>
-      </c>
-      <c r="D34" t="s">
-        <v>171</v>
-      </c>
-      <c r="J34" t="s">
-        <v>172</v>
-      </c>
-      <c r="K34" t="s">
-        <v>236</v>
-      </c>
-      <c r="L34" t="s">
-        <v>108</v>
-      </c>
-      <c r="M34" t="s">
-        <v>145</v>
-      </c>
-      <c r="N34" t="s">
-        <v>146</v>
-      </c>
       <c r="O34" t="s">
+        <v>143</v>
+      </c>
+      <c r="P34" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q34" t="s">
         <v>111</v>
       </c>
-      <c r="P34" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>86</v>
-      </c>
       <c r="R34" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="S34" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="T34" t="s">
-        <v>88</v>
+        <v>113</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V34" t="s">
+        <v>264</v>
+      </c>
+      <c r="W34" t="s">
+        <v>265</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35">
         <v>89</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>266</v>
       </c>
       <c r="C35" t="s">
-        <v>201</v>
+        <v>266</v>
       </c>
       <c r="D35" t="s">
-        <v>173</v>
+        <v>267</v>
       </c>
       <c r="J35" t="s">
-        <v>174</v>
+        <v>268</v>
       </c>
       <c r="K35" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L35" t="s">
-        <v>175</v>
+        <v>269</v>
       </c>
       <c r="M35" t="s">
-        <v>176</v>
+        <v>270</v>
       </c>
       <c r="N35" t="s">
-        <v>177</v>
+        <v>271</v>
       </c>
       <c r="O35" t="s">
-        <v>178</v>
+        <v>272</v>
       </c>
       <c r="P35" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q35" t="s">
-        <v>175</v>
+        <v>269</v>
       </c>
       <c r="R35" t="s">
-        <v>176</v>
+        <v>270</v>
       </c>
       <c r="S35" t="s">
-        <v>177</v>
+        <v>271</v>
       </c>
       <c r="T35" t="s">
-        <v>178</v>
+        <v>272</v>
+      </c>
+      <c r="U35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V35" t="s">
+        <v>273</v>
+      </c>
+      <c r="W35" t="s">
+        <v>274</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23">
       <c r="A36">
         <v>90</v>
       </c>
       <c r="B36" t="s">
-        <v>202</v>
+        <v>275</v>
       </c>
       <c r="C36" t="s">
-        <v>202</v>
+        <v>275</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>276</v>
       </c>
       <c r="J36" t="s">
-        <v>180</v>
+        <v>277</v>
       </c>
       <c r="K36" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L36" t="s">
-        <v>157</v>
+        <v>226</v>
       </c>
       <c r="M36" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="N36" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="O36" t="s">
-        <v>158</v>
+        <v>227</v>
       </c>
       <c r="P36" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q36" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="R36" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="S36" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="T36" t="s">
-        <v>62</v>
+        <v>80</v>
+      </c>
+      <c r="U36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V36" t="s">
+        <v>278</v>
+      </c>
+      <c r="W36" t="s">
+        <v>279</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23">
       <c r="A37">
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>203</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
-        <v>203</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>181</v>
+        <v>280</v>
       </c>
       <c r="J37" t="s">
-        <v>182</v>
+        <v>281</v>
       </c>
       <c r="K37" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="L37" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="M37" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="N37" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="O37" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="P37" t="s">
-        <v>236</v>
+        <v>26</v>
       </c>
       <c r="Q37" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="R37" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="S37" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="T37" t="s">
-        <v>62</v>
+        <v>80</v>
+      </c>
+      <c r="U37" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V37" t="s">
+        <v>282</v>
+      </c>
+      <c r="W37" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>